<commit_message>
- Update the P4 chart comparison.
</commit_message>
<xml_diff>
--- a/graph/Empirical Comparison.xlsx
+++ b/graph/Empirical Comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lutaiphong/Projects/MIU/CS522-BD-Hadoop/graph/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEB5971-8471-E441-A5E2-44F25B61766D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DD981C-A575-814D-99EF-F34F6F99FF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18040" windowHeight="24000" xr2:uid="{575DB921-1493-674F-B097-146AF70A5FF8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24060" windowHeight="24000" xr2:uid="{575DB921-1493-674F-B097-146AF70A5FF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -291,34 +291,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>132</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -404,31 +404,31 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>48</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>54</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>60</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>66</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -788,34 +788,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>437</c:v>
+                  <c:v>617</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>434</c:v>
+                  <c:v>867</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>439</c:v>
+                  <c:v>1267</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>443</c:v>
+                  <c:v>1551</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>441</c:v>
+                  <c:v>1832</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>443</c:v>
+                  <c:v>1988</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>433</c:v>
+                  <c:v>1699</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>445</c:v>
+                  <c:v>1393</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>442</c:v>
+                  <c:v>1145</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>447</c:v>
+                  <c:v>874</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -898,34 +898,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>643</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>904</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>1138</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>1424</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36</c:v>
+                  <c:v>1698</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42</c:v>
+                  <c:v>1968</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>48</c:v>
+                  <c:v>1845</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>54</c:v>
+                  <c:v>1589</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>60</c:v>
+                  <c:v>1323</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>66</c:v>
+                  <c:v>1063</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2692,7 +2692,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="158" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2754,34 +2754,34 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D3">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="E3">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="F3">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="G3">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="H3">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="I3">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="J3">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="K3">
-        <v>10</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -2792,31 +2792,31 @@
         <v>12</v>
       </c>
       <c r="C4">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D4">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E4">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F4">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G4">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H4">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="I4">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="J4">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="K4">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="19" x14ac:dyDescent="0.25">
@@ -2873,34 +2873,34 @@
         <v>0</v>
       </c>
       <c r="B8">
-        <v>437</v>
+        <v>617</v>
       </c>
       <c r="C8">
-        <v>434</v>
+        <v>867</v>
       </c>
       <c r="D8">
-        <v>439</v>
+        <v>1267</v>
       </c>
       <c r="E8">
-        <v>443</v>
+        <v>1551</v>
       </c>
       <c r="F8">
-        <v>441</v>
+        <v>1832</v>
       </c>
       <c r="G8">
-        <v>443</v>
+        <v>1988</v>
       </c>
       <c r="H8">
-        <v>433</v>
+        <v>1699</v>
       </c>
       <c r="I8">
-        <v>445</v>
+        <v>1393</v>
       </c>
       <c r="J8">
-        <v>442</v>
+        <v>1145</v>
       </c>
       <c r="K8">
-        <v>447</v>
+        <v>874</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -2908,34 +2908,34 @@
         <v>1</v>
       </c>
       <c r="B9">
-        <v>12</v>
+        <v>643</v>
       </c>
       <c r="C9">
-        <v>18</v>
+        <v>904</v>
       </c>
       <c r="D9">
-        <v>24</v>
+        <v>1138</v>
       </c>
       <c r="E9">
-        <v>30</v>
+        <v>1424</v>
       </c>
       <c r="F9">
-        <v>36</v>
+        <v>1698</v>
       </c>
       <c r="G9">
-        <v>42</v>
+        <v>1968</v>
       </c>
       <c r="H9">
-        <v>48</v>
+        <v>1845</v>
       </c>
       <c r="I9">
-        <v>54</v>
+        <v>1589</v>
       </c>
       <c r="J9">
-        <v>60</v>
+        <v>1323</v>
       </c>
       <c r="K9">
-        <v>66</v>
+        <v>1063</v>
       </c>
     </row>
   </sheetData>

</xml_diff>